<commit_message>
HNRS-2 DPE and DD for HNRS
</commit_message>
<xml_diff>
--- a/analyst/Ines/rmonize/data_dictionary/DD_HNRS_INES.xlsx
+++ b/analyst/Ines/rmonize/data_dictionary/DD_HNRS_INES.xlsx
@@ -1,22 +1,110 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perrar\Documents\Perrar\NFDI4Health\TA5_1\use-cases-harmonisation\analyst\Ines\rmonize\data_dictionary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>valueType</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>TRIGN</t>
+  </si>
+  <si>
+    <t>CHOLN</t>
+  </si>
+  <si>
+    <t>LDLN</t>
+  </si>
+  <si>
+    <t>HDLN</t>
+  </si>
+  <si>
+    <t>BMI</t>
+  </si>
+  <si>
+    <t>BMI_T2</t>
+  </si>
+  <si>
+    <t>Taille_T2</t>
+  </si>
+  <si>
+    <t>Taille</t>
+  </si>
+  <si>
+    <t>Huefte</t>
+  </si>
+  <si>
+    <t>Huefte_T2</t>
+  </si>
+  <si>
+    <t>Alter_T2</t>
+  </si>
+  <si>
+    <t>Triglyceride</t>
+  </si>
+  <si>
+    <t>Cholesterin</t>
+  </si>
+  <si>
+    <t>LDL</t>
+  </si>
+  <si>
+    <t>HDL</t>
+  </si>
+  <si>
+    <t>BMI (T0)</t>
+  </si>
+  <si>
+    <t>BMI (T2)</t>
+  </si>
+  <si>
+    <t>Taillenumfang</t>
+  </si>
+  <si>
+    <t>Hüftumfang</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,6 +119,31 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -53,22 +166,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -110,7 +239,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +271,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +306,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,33 +482,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>valueType</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -386,28 +635,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>